<commit_message>
Air simulation step is nearly done, on water step is working:wq
</commit_message>
<xml_diff>
--- a/Utils/TerrainGenerator/MaxHumidity.xlsx
+++ b/Utils/TerrainGenerator/MaxHumidity.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\firstwxgame\Utils\TerrainGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BDD995-3BD3-44C9-B5A6-00F81AA744BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4FB152-4E25-43E9-9A34-1C62AD4BF576}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{471F85BF-902E-4586-80B9-4B5B383405DC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" activeTab="1" xr2:uid="{471F85BF-902E-4586-80B9-4B5B383405DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hustota" sheetId="2" r:id="rId2"/>
+    <sheet name="Testing" sheetId="3" r:id="rId2"/>
+    <sheet name="Hustota" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,13 +27,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Hustota0</t>
+  </si>
+  <si>
+    <t>Tlak0</t>
+  </si>
+  <si>
+    <t>Gr.zrych.</t>
+  </si>
+  <si>
+    <t>Změna výšky</t>
+  </si>
+  <si>
+    <t>Tlak v danné výšce</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -87,10 +104,10 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C586E7-8ADA-4D9A-B679-1A0B43412F7F}">
   <dimension ref="A1:U201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="F46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
@@ -9832,6 +9849,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA48EE6-BD86-4350-8EBE-8FBE6448F138}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.25</v>
+      </c>
+      <c r="B2">
+        <v>73161.56</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>-2500</v>
+      </c>
+      <c r="F2">
+        <f>B2*EXP(-($A$2*$C$2*D2)/B2)</f>
+        <v>112146.60852011929</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>100000</v>
+      </c>
+      <c r="D3">
+        <v>2500</v>
+      </c>
+      <c r="F3">
+        <f>B3*EXP(-($A$2*$C$2*D3)/B3)</f>
+        <v>73161.562894664181</v>
+      </c>
+      <c r="H3">
+        <f>(F3/B3)*15</f>
+        <v>10.974234434199627</v>
+      </c>
+      <c r="I3">
+        <f>15-0.005*2500</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>100000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>B5/(1 - D5/44330)^5.255</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>100000</v>
+      </c>
+      <c r="D6">
+        <v>2500</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F7" si="0">B6/(1 - D6/44330)^5.255</f>
+        <v>135668.13334930624</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>73709.276844348482</v>
+      </c>
+      <c r="D7">
+        <v>2500</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EA15F4-5792-4461-8A61-7D27691D7842}">
   <dimension ref="A1:H13"/>
   <sheetViews>

</xml_diff>